<commit_message>
Fixed count of members
</commit_message>
<xml_diff>
--- a/before_pass4.xlsx
+++ b/before_pass4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py_apps\KD1662_bot\kd1662\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82F3229B-FD80-4B72-B60F-9B0FE182AD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2E8BC5-C6CE-4B76-9FF9-E7E9A539354B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EFC980CB-5E14-4FAA-A20A-D399F92400F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{EFC980CB-5E14-4FAA-A20A-D399F92400F9}"/>
   </bookViews>
   <sheets>
     <sheet name="2025-06-04" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="289">
   <si>
     <t>Governor Name</t>
   </si>
@@ -907,9 +907,6 @@
   </si>
   <si>
     <t>Governor77933580</t>
-  </si>
-  <si>
-    <t>dead1662</t>
   </si>
 </sst>
 </file>
@@ -1297,9 +1294,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P276"/>
+  <dimension ref="A1:P254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="A265" sqref="A265"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -12824,672 +12823,6 @@
       <c r="N254" s="2"/>
       <c r="O254" s="2"/>
       <c r="P254" s="2"/>
-    </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A255" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B255" s="2">
-        <v>186268387</v>
-      </c>
-      <c r="C255" s="2">
-        <v>117786</v>
-      </c>
-      <c r="D255" s="2"/>
-      <c r="E255" s="2">
-        <v>0</v>
-      </c>
-      <c r="F255" s="2"/>
-      <c r="G255" s="2"/>
-      <c r="H255" s="2">
-        <v>0</v>
-      </c>
-      <c r="I255" s="2"/>
-      <c r="J255" s="2">
-        <v>0</v>
-      </c>
-      <c r="K255" s="2">
-        <v>0</v>
-      </c>
-      <c r="L255" s="2">
-        <v>19</v>
-      </c>
-      <c r="M255" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="N255" s="2"/>
-      <c r="O255" s="2"/>
-      <c r="P255" s="2"/>
-    </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A256" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B256" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C256" s="2">
-        <v>0</v>
-      </c>
-      <c r="D256" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E256" s="2">
-        <v>7</v>
-      </c>
-      <c r="F256" s="2"/>
-      <c r="G256" s="2"/>
-      <c r="H256" s="2"/>
-      <c r="I256" s="2"/>
-      <c r="J256" s="2"/>
-      <c r="K256" s="2"/>
-      <c r="L256" s="2"/>
-      <c r="M256" s="2"/>
-      <c r="N256" s="2"/>
-      <c r="O256" s="2"/>
-      <c r="P256" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A257" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B257" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C257" s="2">
-        <v>0</v>
-      </c>
-      <c r="D257" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E257" s="2">
-        <v>7</v>
-      </c>
-      <c r="F257" s="2"/>
-      <c r="G257" s="2"/>
-      <c r="H257" s="2"/>
-      <c r="I257" s="2"/>
-      <c r="J257" s="2"/>
-      <c r="K257" s="2"/>
-      <c r="L257" s="2"/>
-      <c r="M257" s="2"/>
-      <c r="N257" s="2"/>
-      <c r="O257" s="2"/>
-      <c r="P257" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A258" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B258" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C258" s="2">
-        <v>0</v>
-      </c>
-      <c r="D258" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E258" s="2">
-        <v>7</v>
-      </c>
-      <c r="F258" s="2"/>
-      <c r="G258" s="2"/>
-      <c r="H258" s="2"/>
-      <c r="I258" s="2"/>
-      <c r="J258" s="2"/>
-      <c r="K258" s="2"/>
-      <c r="L258" s="2"/>
-      <c r="M258" s="2"/>
-      <c r="N258" s="2"/>
-      <c r="O258" s="2"/>
-      <c r="P258" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A259" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B259" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C259" s="2">
-        <v>0</v>
-      </c>
-      <c r="D259" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E259" s="2">
-        <v>7</v>
-      </c>
-      <c r="F259" s="2"/>
-      <c r="G259" s="2"/>
-      <c r="H259" s="2"/>
-      <c r="I259" s="2"/>
-      <c r="J259" s="2"/>
-      <c r="K259" s="2"/>
-      <c r="L259" s="2"/>
-      <c r="M259" s="2"/>
-      <c r="N259" s="2"/>
-      <c r="O259" s="2"/>
-      <c r="P259" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A260" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B260" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C260" s="2">
-        <v>0</v>
-      </c>
-      <c r="D260" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E260" s="2">
-        <v>7</v>
-      </c>
-      <c r="F260" s="2"/>
-      <c r="G260" s="2"/>
-      <c r="H260" s="2"/>
-      <c r="I260" s="2"/>
-      <c r="J260" s="2"/>
-      <c r="K260" s="2"/>
-      <c r="L260" s="2"/>
-      <c r="M260" s="2"/>
-      <c r="N260" s="2"/>
-      <c r="O260" s="2"/>
-      <c r="P260" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A261" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B261" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C261" s="2">
-        <v>0</v>
-      </c>
-      <c r="D261" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E261" s="2">
-        <v>7</v>
-      </c>
-      <c r="F261" s="2"/>
-      <c r="G261" s="2"/>
-      <c r="H261" s="2"/>
-      <c r="I261" s="2"/>
-      <c r="J261" s="2"/>
-      <c r="K261" s="2"/>
-      <c r="L261" s="2"/>
-      <c r="M261" s="2"/>
-      <c r="N261" s="2"/>
-      <c r="O261" s="2"/>
-      <c r="P261" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A262" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B262" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C262" s="2">
-        <v>0</v>
-      </c>
-      <c r="D262" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E262" s="2">
-        <v>7</v>
-      </c>
-      <c r="F262" s="2"/>
-      <c r="G262" s="2"/>
-      <c r="H262" s="2"/>
-      <c r="I262" s="2"/>
-      <c r="J262" s="2"/>
-      <c r="K262" s="2"/>
-      <c r="L262" s="2"/>
-      <c r="M262" s="2"/>
-      <c r="N262" s="2"/>
-      <c r="O262" s="2"/>
-      <c r="P262" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A263" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B263" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C263" s="2">
-        <v>0</v>
-      </c>
-      <c r="D263" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E263" s="2">
-        <v>7</v>
-      </c>
-      <c r="F263" s="2"/>
-      <c r="G263" s="2"/>
-      <c r="H263" s="2"/>
-      <c r="I263" s="2"/>
-      <c r="J263" s="2"/>
-      <c r="K263" s="2"/>
-      <c r="L263" s="2"/>
-      <c r="M263" s="2"/>
-      <c r="N263" s="2"/>
-      <c r="O263" s="2"/>
-      <c r="P263" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A264" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B264" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C264" s="2">
-        <v>0</v>
-      </c>
-      <c r="D264" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E264" s="2">
-        <v>7</v>
-      </c>
-      <c r="F264" s="2"/>
-      <c r="G264" s="2"/>
-      <c r="H264" s="2"/>
-      <c r="I264" s="2"/>
-      <c r="J264" s="2"/>
-      <c r="K264" s="2"/>
-      <c r="L264" s="2"/>
-      <c r="M264" s="2"/>
-      <c r="N264" s="2"/>
-      <c r="O264" s="2"/>
-      <c r="P264" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A265" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B265" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C265" s="2">
-        <v>0</v>
-      </c>
-      <c r="D265" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E265" s="2">
-        <v>7</v>
-      </c>
-      <c r="F265" s="2"/>
-      <c r="G265" s="2"/>
-      <c r="H265" s="2"/>
-      <c r="I265" s="2"/>
-      <c r="J265" s="2"/>
-      <c r="K265" s="2"/>
-      <c r="L265" s="2"/>
-      <c r="M265" s="2"/>
-      <c r="N265" s="2"/>
-      <c r="O265" s="2"/>
-      <c r="P265" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A266" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B266" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C266" s="2">
-        <v>0</v>
-      </c>
-      <c r="D266" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E266" s="2">
-        <v>7</v>
-      </c>
-      <c r="F266" s="2"/>
-      <c r="G266" s="2"/>
-      <c r="H266" s="2"/>
-      <c r="I266" s="2"/>
-      <c r="J266" s="2"/>
-      <c r="K266" s="2"/>
-      <c r="L266" s="2"/>
-      <c r="M266" s="2"/>
-      <c r="N266" s="2"/>
-      <c r="O266" s="2"/>
-      <c r="P266" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A267" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B267" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C267" s="2">
-        <v>0</v>
-      </c>
-      <c r="D267" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E267" s="2">
-        <v>7</v>
-      </c>
-      <c r="F267" s="2"/>
-      <c r="G267" s="2"/>
-      <c r="H267" s="2"/>
-      <c r="I267" s="2"/>
-      <c r="J267" s="2"/>
-      <c r="K267" s="2"/>
-      <c r="L267" s="2"/>
-      <c r="M267" s="2"/>
-      <c r="N267" s="2"/>
-      <c r="O267" s="2"/>
-      <c r="P267" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A268" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B268" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C268" s="2">
-        <v>0</v>
-      </c>
-      <c r="D268" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E268" s="2">
-        <v>7</v>
-      </c>
-      <c r="F268" s="2"/>
-      <c r="G268" s="2"/>
-      <c r="H268" s="2"/>
-      <c r="I268" s="2"/>
-      <c r="J268" s="2"/>
-      <c r="K268" s="2"/>
-      <c r="L268" s="2"/>
-      <c r="M268" s="2"/>
-      <c r="N268" s="2"/>
-      <c r="O268" s="2"/>
-      <c r="P268" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A269" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B269" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C269" s="2">
-        <v>0</v>
-      </c>
-      <c r="D269" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E269" s="2">
-        <v>7</v>
-      </c>
-      <c r="F269" s="2"/>
-      <c r="G269" s="2"/>
-      <c r="H269" s="2"/>
-      <c r="I269" s="2"/>
-      <c r="J269" s="2"/>
-      <c r="K269" s="2"/>
-      <c r="L269" s="2"/>
-      <c r="M269" s="2"/>
-      <c r="N269" s="2"/>
-      <c r="O269" s="2"/>
-      <c r="P269" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A270" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B270" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C270" s="2">
-        <v>0</v>
-      </c>
-      <c r="D270" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E270" s="2">
-        <v>7</v>
-      </c>
-      <c r="F270" s="2"/>
-      <c r="G270" s="2"/>
-      <c r="H270" s="2"/>
-      <c r="I270" s="2"/>
-      <c r="J270" s="2"/>
-      <c r="K270" s="2"/>
-      <c r="L270" s="2"/>
-      <c r="M270" s="2"/>
-      <c r="N270" s="2"/>
-      <c r="O270" s="2"/>
-      <c r="P270" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A271" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B271" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C271" s="2">
-        <v>0</v>
-      </c>
-      <c r="D271" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E271" s="2">
-        <v>7</v>
-      </c>
-      <c r="F271" s="2"/>
-      <c r="G271" s="2"/>
-      <c r="H271" s="2"/>
-      <c r="I271" s="2"/>
-      <c r="J271" s="2"/>
-      <c r="K271" s="2"/>
-      <c r="L271" s="2"/>
-      <c r="M271" s="2"/>
-      <c r="N271" s="2"/>
-      <c r="O271" s="2"/>
-      <c r="P271" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A272" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B272" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C272" s="2">
-        <v>0</v>
-      </c>
-      <c r="D272" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E272" s="2">
-        <v>7</v>
-      </c>
-      <c r="F272" s="2"/>
-      <c r="G272" s="2"/>
-      <c r="H272" s="2"/>
-      <c r="I272" s="2"/>
-      <c r="J272" s="2"/>
-      <c r="K272" s="2"/>
-      <c r="L272" s="2"/>
-      <c r="M272" s="2"/>
-      <c r="N272" s="2"/>
-      <c r="O272" s="2"/>
-      <c r="P272" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A273" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B273" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C273" s="2">
-        <v>0</v>
-      </c>
-      <c r="D273" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E273" s="2">
-        <v>7</v>
-      </c>
-      <c r="F273" s="2"/>
-      <c r="G273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="I273" s="2"/>
-      <c r="J273" s="2"/>
-      <c r="K273" s="2"/>
-      <c r="L273" s="2"/>
-      <c r="M273" s="2"/>
-      <c r="N273" s="2"/>
-      <c r="O273" s="2"/>
-      <c r="P273" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A274" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B274" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C274" s="2">
-        <v>0</v>
-      </c>
-      <c r="D274" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E274" s="2">
-        <v>7</v>
-      </c>
-      <c r="F274" s="2"/>
-      <c r="G274" s="2"/>
-      <c r="H274" s="2"/>
-      <c r="I274" s="2"/>
-      <c r="J274" s="2"/>
-      <c r="K274" s="2"/>
-      <c r="L274" s="2"/>
-      <c r="M274" s="2"/>
-      <c r="N274" s="2"/>
-      <c r="O274" s="2"/>
-      <c r="P274" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A275" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B275" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C275" s="2">
-        <v>0</v>
-      </c>
-      <c r="D275" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E275" s="2">
-        <v>7</v>
-      </c>
-      <c r="F275" s="2"/>
-      <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="2"/>
-      <c r="J275" s="2"/>
-      <c r="K275" s="2"/>
-      <c r="L275" s="2"/>
-      <c r="M275" s="2"/>
-      <c r="N275" s="2"/>
-      <c r="O275" s="2"/>
-      <c r="P275" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A276" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B276" s="2">
-        <v>201914393</v>
-      </c>
-      <c r="C276" s="2">
-        <v>0</v>
-      </c>
-      <c r="D276" s="2">
-        <v>45452</v>
-      </c>
-      <c r="E276" s="2">
-        <v>7</v>
-      </c>
-      <c r="F276" s="2"/>
-      <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
-      <c r="I276" s="2"/>
-      <c r="J276" s="2"/>
-      <c r="K276" s="2"/>
-      <c r="L276" s="2"/>
-      <c r="M276" s="2"/>
-      <c r="N276" s="2"/>
-      <c r="O276" s="2"/>
-      <c r="P276" s="2">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>